<commit_message>
fix: Switch to flyqdrone.in custom domain for all links
</commit_message>
<xml_diff>
--- a/FLYQ_Customer_Orders_2026-01-24.xlsx
+++ b/FLYQ_Customer_Orders_2026-01-24.xlsx
@@ -546,10 +546,10 @@
         <v>N/A</v>
       </c>
       <c r="S2" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T2" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK176927506422962EM7G</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK176927506422962EM7G</v>
       </c>
       <c r="U2" t="str">
         <v>24/1/2026</v>
@@ -611,10 +611,10 @@
         <v>N/A</v>
       </c>
       <c r="S3" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T3" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064365KL6TX1</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064365KL6TX1</v>
       </c>
       <c r="U3" t="str">
         <v>24/1/2026</v>
@@ -676,10 +676,10 @@
         <v>N/A</v>
       </c>
       <c r="S4" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T4" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064423NLJ7HD</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064423NLJ7HD</v>
       </c>
       <c r="U4" t="str">
         <v>24/1/2026</v>
@@ -741,10 +741,10 @@
         <v>N/A</v>
       </c>
       <c r="S5" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T5" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750644801BFUUV</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750644801BFUUV</v>
       </c>
       <c r="U5" t="str">
         <v>24/1/2026</v>
@@ -806,10 +806,10 @@
         <v>N/A</v>
       </c>
       <c r="S6" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T6" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064524EU8VFJ</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064524EU8VFJ</v>
       </c>
       <c r="U6" t="str">
         <v>24/1/2026</v>
@@ -871,10 +871,10 @@
         <v>N/A</v>
       </c>
       <c r="S7" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T7" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750645778LE488</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750645778LE488</v>
       </c>
       <c r="U7" t="str">
         <v>24/1/2026</v>
@@ -936,10 +936,10 @@
         <v>N/A</v>
       </c>
       <c r="S8" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T8" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064617ENH831</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064617ENH831</v>
       </c>
       <c r="U8" t="str">
         <v>24/1/2026</v>
@@ -1001,10 +1001,10 @@
         <v>N/A</v>
       </c>
       <c r="S9" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T9" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750646573HU7QT</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750646573HU7QT</v>
       </c>
       <c r="U9" t="str">
         <v>24/1/2026</v>
@@ -1066,10 +1066,10 @@
         <v>N/A</v>
       </c>
       <c r="S10" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T10" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064713IHVOY8</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064713IHVOY8</v>
       </c>
       <c r="U10" t="str">
         <v>24/1/2026</v>
@@ -1131,10 +1131,10 @@
         <v>N/A</v>
       </c>
       <c r="S11" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T11" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064754PL9Y4S</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064754PL9Y4S</v>
       </c>
       <c r="U11" t="str">
         <v>24/1/2026</v>
@@ -1196,10 +1196,10 @@
         <v>N/A</v>
       </c>
       <c r="S12" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T12" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK176927506480670S96X</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK176927506480670S96X</v>
       </c>
       <c r="U12" t="str">
         <v>24/1/2026</v>
@@ -1261,10 +1261,10 @@
         <v>N/A</v>
       </c>
       <c r="S13" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T13" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064852HLVD2M</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064852HLVD2M</v>
       </c>
       <c r="U13" t="str">
         <v>24/1/2026</v>
@@ -1326,10 +1326,10 @@
         <v>N/A</v>
       </c>
       <c r="S14" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T14" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275064976E1F2LU</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275064976E1F2LU</v>
       </c>
       <c r="U14" t="str">
         <v>24/1/2026</v>
@@ -1391,10 +1391,10 @@
         <v>N/A</v>
       </c>
       <c r="S15" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T15" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065070AXOQPE</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065070AXOQPE</v>
       </c>
       <c r="U15" t="str">
         <v>24/1/2026</v>
@@ -1456,10 +1456,10 @@
         <v>N/A</v>
       </c>
       <c r="S16" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T16" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065124FUZ9IK</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065124FUZ9IK</v>
       </c>
       <c r="U16" t="str">
         <v>24/1/2026</v>
@@ -1521,10 +1521,10 @@
         <v>N/A</v>
       </c>
       <c r="S17" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T17" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750652165SUEND</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750652165SUEND</v>
       </c>
       <c r="U17" t="str">
         <v>24/1/2026</v>
@@ -1586,10 +1586,10 @@
         <v>N/A</v>
       </c>
       <c r="S18" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T18" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK176927506528173YRPA</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK176927506528173YRPA</v>
       </c>
       <c r="U18" t="str">
         <v>24/1/2026</v>
@@ -1651,10 +1651,10 @@
         <v>N/A</v>
       </c>
       <c r="S19" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T19" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065354EPTUTU</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065354EPTUTU</v>
       </c>
       <c r="U19" t="str">
         <v>24/1/2026</v>
@@ -1716,10 +1716,10 @@
         <v>N/A</v>
       </c>
       <c r="S20" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T20" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065404RHWLKH</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065404RHWLKH</v>
       </c>
       <c r="U20" t="str">
         <v>24/1/2026</v>
@@ -1781,10 +1781,10 @@
         <v>N/A</v>
       </c>
       <c r="S21" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T21" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065460CM0GGM</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065460CM0GGM</v>
       </c>
       <c r="U21" t="str">
         <v>24/1/2026</v>
@@ -1846,10 +1846,10 @@
         <v>N/A</v>
       </c>
       <c r="S22" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T22" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065515DXK3M0</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065515DXK3M0</v>
       </c>
       <c r="U22" t="str">
         <v>24/1/2026</v>
@@ -1911,10 +1911,10 @@
         <v>N/A</v>
       </c>
       <c r="S23" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T23" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065572XT3WXY</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065572XT3WXY</v>
       </c>
       <c r="U23" t="str">
         <v>24/1/2026</v>
@@ -1976,10 +1976,10 @@
         <v>N/A</v>
       </c>
       <c r="S24" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T24" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065621V4AM45</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065621V4AM45</v>
       </c>
       <c r="U24" t="str">
         <v>24/1/2026</v>
@@ -2041,10 +2041,10 @@
         <v>N/A</v>
       </c>
       <c r="S25" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T25" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065675A6IO64</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065675A6IO64</v>
       </c>
       <c r="U25" t="str">
         <v>24/1/2026</v>
@@ -2106,10 +2106,10 @@
         <v>N/A</v>
       </c>
       <c r="S26" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T26" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK176927506577262EJM4</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK176927506577262EJM4</v>
       </c>
       <c r="U26" t="str">
         <v>24/1/2026</v>
@@ -2171,10 +2171,10 @@
         <v>N/A</v>
       </c>
       <c r="S27" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T27" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750658473TWAPW</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750658473TWAPW</v>
       </c>
       <c r="U27" t="str">
         <v>24/1/2026</v>
@@ -2236,10 +2236,10 @@
         <v>N/A</v>
       </c>
       <c r="S28" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T28" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065886AS0W4E</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065886AS0W4E</v>
       </c>
       <c r="U28" t="str">
         <v>24/1/2026</v>
@@ -2301,10 +2301,10 @@
         <v>N/A</v>
       </c>
       <c r="S29" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T29" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065925V2QUKN</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065925V2QUKN</v>
       </c>
       <c r="U29" t="str">
         <v>24/1/2026</v>
@@ -2366,10 +2366,10 @@
         <v>N/A</v>
       </c>
       <c r="S30" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T30" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065961AJU0R2</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065961AJU0R2</v>
       </c>
       <c r="U30" t="str">
         <v>24/1/2026</v>
@@ -2431,10 +2431,10 @@
         <v>N/A</v>
       </c>
       <c r="S31" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T31" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275065995E1F6HC</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275065995E1F6HC</v>
       </c>
       <c r="U31" t="str">
         <v>24/1/2026</v>
@@ -2496,10 +2496,10 @@
         <v>N/A</v>
       </c>
       <c r="S32" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T32" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066033JRK9S2</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066033JRK9S2</v>
       </c>
       <c r="U32" t="str">
         <v>24/1/2026</v>
@@ -2561,10 +2561,10 @@
         <v>N/A</v>
       </c>
       <c r="S33" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T33" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066072N3LEB0</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066072N3LEB0</v>
       </c>
       <c r="U33" t="str">
         <v>24/1/2026</v>
@@ -2626,10 +2626,10 @@
         <v>N/A</v>
       </c>
       <c r="S34" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T34" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066111BZZI7D</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066111BZZI7D</v>
       </c>
       <c r="U34" t="str">
         <v>24/1/2026</v>
@@ -2691,10 +2691,10 @@
         <v>N/A</v>
       </c>
       <c r="S35" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T35" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK176927506615728AQ3K</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK176927506615728AQ3K</v>
       </c>
       <c r="U35" t="str">
         <v>24/1/2026</v>
@@ -2756,10 +2756,10 @@
         <v>N/A</v>
       </c>
       <c r="S36" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T36" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066202DGYEYN</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066202DGYEYN</v>
       </c>
       <c r="U36" t="str">
         <v>24/1/2026</v>
@@ -2821,10 +2821,10 @@
         <v>N/A</v>
       </c>
       <c r="S37" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T37" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750662458QN6IX</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750662458QN6IX</v>
       </c>
       <c r="U37" t="str">
         <v>24/1/2026</v>
@@ -2886,10 +2886,10 @@
         <v>N/A</v>
       </c>
       <c r="S38" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T38" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066291Z925RG</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066291Z925RG</v>
       </c>
       <c r="U38" t="str">
         <v>24/1/2026</v>
@@ -2951,10 +2951,10 @@
         <v>N/A</v>
       </c>
       <c r="S39" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T39" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066341DAENIO</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066341DAENIO</v>
       </c>
       <c r="U39" t="str">
         <v>24/1/2026</v>
@@ -3016,10 +3016,10 @@
         <v>N/A</v>
       </c>
       <c r="S40" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T40" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750663860XGSOV</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750663860XGSOV</v>
       </c>
       <c r="U40" t="str">
         <v>24/1/2026</v>
@@ -3081,10 +3081,10 @@
         <v>N/A</v>
       </c>
       <c r="S41" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T41" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066441W8PH0G</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066441W8PH0G</v>
       </c>
       <c r="U41" t="str">
         <v>24/1/2026</v>
@@ -3148,10 +3148,10 @@
         <v>N/A</v>
       </c>
       <c r="S42" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T42" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066502EMA3XR</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066502EMA3XR</v>
       </c>
       <c r="U42" t="str">
         <v>24/1/2026</v>
@@ -3213,10 +3213,10 @@
         <v>N/A</v>
       </c>
       <c r="S43" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T43" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066551XPLJ8T</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066551XPLJ8T</v>
       </c>
       <c r="U43" t="str">
         <v>24/1/2026</v>
@@ -3278,10 +3278,10 @@
         <v>N/A</v>
       </c>
       <c r="S44" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T44" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066612YFNT75</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066612YFNT75</v>
       </c>
       <c r="U44" t="str">
         <v>24/1/2026</v>
@@ -3344,10 +3344,10 @@
         <v>N/A</v>
       </c>
       <c r="S45" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T45" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750666611CT0GY</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750666611CT0GY</v>
       </c>
       <c r="U45" t="str">
         <v>24/1/2026</v>
@@ -3409,10 +3409,10 @@
         <v>N/A</v>
       </c>
       <c r="S46" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T46" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066711EIYK56</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066711EIYK56</v>
       </c>
       <c r="U46" t="str">
         <v>24/1/2026</v>
@@ -3474,10 +3474,10 @@
         <v>N/A</v>
       </c>
       <c r="S47" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T47" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066762XPWHNE</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066762XPWHNE</v>
       </c>
       <c r="U47" t="str">
         <v>24/1/2026</v>
@@ -3539,10 +3539,10 @@
         <v>N/A</v>
       </c>
       <c r="S48" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T48" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066814JACH9M</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066814JACH9M</v>
       </c>
       <c r="U48" t="str">
         <v>24/1/2026</v>
@@ -3604,10 +3604,10 @@
         <v>N/A</v>
       </c>
       <c r="S49" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T49" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK176927506686049ZRIF</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK176927506686049ZRIF</v>
       </c>
       <c r="U49" t="str">
         <v>24/1/2026</v>
@@ -3669,10 +3669,10 @@
         <v>N/A</v>
       </c>
       <c r="S50" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T50" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066933ALKQ5E</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066933ALKQ5E</v>
       </c>
       <c r="U50" t="str">
         <v>24/1/2026</v>
@@ -3734,10 +3734,10 @@
         <v>N/A</v>
       </c>
       <c r="S51" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T51" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275066979J9R0BE</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275066979J9R0BE</v>
       </c>
       <c r="U51" t="str">
         <v>24/1/2026</v>
@@ -3799,10 +3799,10 @@
         <v>N/A</v>
       </c>
       <c r="S52" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T52" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK176927506703186VHC4</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK176927506703186VHC4</v>
       </c>
       <c r="U52" t="str">
         <v>24/1/2026</v>
@@ -3864,10 +3864,10 @@
         <v>N/A</v>
       </c>
       <c r="S53" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T53" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067093PQFO6Z</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067093PQFO6Z</v>
       </c>
       <c r="U53" t="str">
         <v>24/1/2026</v>
@@ -3929,10 +3929,10 @@
         <v>N/A</v>
       </c>
       <c r="S54" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T54" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750671465YH9Q2</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750671465YH9Q2</v>
       </c>
       <c r="U54" t="str">
         <v>24/1/2026</v>
@@ -3994,10 +3994,10 @@
         <v>N/A</v>
       </c>
       <c r="S55" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T55" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067202VKPMQ1</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067202VKPMQ1</v>
       </c>
       <c r="U55" t="str">
         <v>24/1/2026</v>
@@ -4059,10 +4059,10 @@
         <v>N/A</v>
       </c>
       <c r="S56" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T56" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067248Z1LTTG</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067248Z1LTTG</v>
       </c>
       <c r="U56" t="str">
         <v>24/1/2026</v>
@@ -4124,10 +4124,10 @@
         <v>N/A</v>
       </c>
       <c r="S57" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T57" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067290LVU480</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067290LVU480</v>
       </c>
       <c r="U57" t="str">
         <v>24/1/2026</v>
@@ -4189,10 +4189,10 @@
         <v>N/A</v>
       </c>
       <c r="S58" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T58" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067386Q8Q5DI</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067386Q8Q5DI</v>
       </c>
       <c r="U58" t="str">
         <v>24/1/2026</v>
@@ -4255,10 +4255,10 @@
         <v>N/A</v>
       </c>
       <c r="S59" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T59" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067443E2ZLTQ</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067443E2ZLTQ</v>
       </c>
       <c r="U59" t="str">
         <v>24/1/2026</v>
@@ -4320,10 +4320,10 @@
         <v>N/A</v>
       </c>
       <c r="S60" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T60" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067489RPK787</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067489RPK787</v>
       </c>
       <c r="U60" t="str">
         <v>24/1/2026</v>
@@ -4385,10 +4385,10 @@
         <v>N/A</v>
       </c>
       <c r="S61" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T61" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067551VVYFYX</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067551VVYFYX</v>
       </c>
       <c r="U61" t="str">
         <v>24/1/2026</v>
@@ -4450,10 +4450,10 @@
         <v>N/A</v>
       </c>
       <c r="S62" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T62" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK17692750676226QPJKQ</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK17692750676226QPJKQ</v>
       </c>
       <c r="U62" t="str">
         <v>24/1/2026</v>
@@ -4515,10 +4515,10 @@
         <v>N/A</v>
       </c>
       <c r="S63" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T63" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067868RNR27W</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067868RNR27W</v>
       </c>
       <c r="U63" t="str">
         <v>24/1/2026</v>
@@ -4581,10 +4581,10 @@
         <v>N/A</v>
       </c>
       <c r="S64" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/login</v>
+        <v>https://flyqdrone.in/login</v>
       </c>
       <c r="T64" t="str">
-        <v>https://df6fc469.flyq-air.pages.dev/track-order?tracking=TRK1769275067928W1CSFW</v>
+        <v>https://flyqdrone.in/track-order?tracking=TRK1769275067928W1CSFW</v>
       </c>
       <c r="U64" t="str">
         <v>24/1/2026</v>

</xml_diff>